<commit_message>
added address column in excel sheets
</commit_message>
<xml_diff>
--- a/mathTransformed/HMPSTT_(2015-06-20)_39_3.xlsx
+++ b/mathTransformed/HMPSTT_(2015-06-20)_39_3.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,11 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>District</t>
         </is>
       </c>
@@ -483,6 +488,11 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>Janata Vidyalay ShiraliBhatkal</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -510,6 +520,11 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t>Assistant TeacherShri KatyayaniHigh School Aversa Ankola</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -537,6 +552,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>Govt. High School NadumaskeriKumta</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -564,6 +584,11 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>Govt. High School GerasoppaHonnavar</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -591,6 +616,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
+          <t>G HS BargiKumta</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -618,6 +648,11 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
+          <t>G H S AllankiHonnavar</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -645,6 +680,11 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t>S P H S MarukeriBhatkal</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -673,6 +713,11 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
+          <t>GunavanteHonnavar</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -700,6 +745,11 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>Gibb Girls High SchoolKumta</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -727,6 +777,11 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
+          <t>Assistant TeacherG H S MundalliBhatkal</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -754,6 +809,11 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
+          <t>Janata Vidyalay Kadatoka Honnavar</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -781,6 +841,11 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
+          <t>Assistant TeacherGHS Santeguli</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
           <t>Kumta Uttara Kannada</t>
         </is>
       </c>
@@ -808,6 +873,11 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>Janata Vidyalaya MudgaKarwar</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -835,6 +905,11 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
+          <t>Assistant TeacherGovt. High SchoolAgragone</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>Ankola Uttara Kannada</t>
         </is>
       </c>
@@ -862,6 +937,11 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
+          <t>H P S JannakadkalHonnavar</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -889,6 +969,11 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
+          <t>Karavali High SchoolBhatakal</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -916,6 +1001,11 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
+          <t>KaremmanavarShree Narayan High School NaitesawarWailwad Karwar</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
           <t>Uttar Kannada</t>
         </is>
       </c>
@@ -943,6 +1033,11 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
+          <t>S S Comp. PU College KavalakkiHonnavar</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -970,6 +1065,11 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
+          <t>Assistant TeacherSharavati High ShoolHonnavar</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -997,6 +1097,11 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
+          <t>Hindu High SchoolKarwar</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1024,6 +1129,11 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
+          <t>G H S VannalliKumta</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1051,6 +1161,11 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
+          <t>Secondary High School AngadiKarwar</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1079,6 +1194,11 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
+          <t>Karwar</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1106,6 +1226,11 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
+          <t>Assistant TeacherG H S TenginagundiBhatkal</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1133,6 +1258,11 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
+          <t>Modern High School HalgaKarwar</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1160,6 +1290,11 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
+          <t>Assistant TeacherSatyagrah SmarakVidyalaya ShetgeriAnkola</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1187,6 +1322,11 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
+          <t>Shivaji Compsite P U ColleggeChitakulaKarwar</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1214,6 +1354,11 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
+          <t>Govt High Scool ChittaraHonnavar</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1241,6 +1386,11 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
+          <t>S K P P U College AreangadiHonnavar</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1268,6 +1418,11 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
+          <t>Govt. High SchoolTodurKarwar</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1295,6 +1450,11 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
+          <t>Govt. High School KalleshwarAnkola</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1322,6 +1482,11 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
+          <t>J V Mirjan KodakaniKumta</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1349,6 +1514,11 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
+          <t>Sadashivagad High School Sadashivagad</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1376,6 +1546,11 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
+          <t>G H S Nelli KeriKumta</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1403,6 +1578,11 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
+          <t>G H S BailurBhatkal</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1430,6 +1610,11 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
+          <t>Assistant TeacherG H S BandarBhatkal</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1457,6 +1642,11 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
+          <t>G H S MankiHonnavar</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
           <t>Uttara Kannada</t>
         </is>
       </c>
@@ -1484,6 +1674,11 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
+          <t>Janata Vidyalaya</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
           <t>Kadwad Karwar Uttara Kannada</t>
         </is>
       </c>
@@ -1510,6 +1705,11 @@
         </is>
       </c>
       <c r="F41" t="inlineStr">
+        <is>
+          <t>Union High SchoolMajaliKarwar</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
         <is>
           <t>Uttara Kannada</t>
         </is>

</xml_diff>

<commit_message>
corrected most names to the official names from website
</commit_message>
<xml_diff>
--- a/mathTransformed/HMPSTT_(2015-06-20)_39_3.xlsx
+++ b/mathTransformed/HMPSTT_(2015-06-20)_39_3.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,7 +493,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -557,7 +557,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -653,7 +653,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -685,7 +685,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -750,7 +750,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -782,7 +782,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -814,7 +814,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -846,7 +846,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Kumta Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -878,7 +878,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -942,7 +942,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -974,7 +974,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Uttar Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1327,7 +1327,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1455,7 +1455,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1519,7 +1519,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1615,7 +1615,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1679,7 +1679,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Kadwad Karwar Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>
@@ -1711,7 +1711,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Uttara Kannada</t>
+          <t>Uttara Kannada (Karwar)</t>
         </is>
       </c>
     </row>

</xml_diff>